<commit_message>
Added Yahoo's Estimated Return
</commit_message>
<xml_diff>
--- a/stockDataFile.xlsx
+++ b/stockDataFile.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,11 @@
           <t>Percent Change</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Yahoo Estimated Return</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -451,17 +456,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>177.49</t>
+          <t>177.70</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+2.58</t>
+          <t>+0.21</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+1.48%</t>
+          <t>+0.12%</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-2%</t>
         </is>
       </c>
     </row>
@@ -473,17 +483,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>138.73</t>
+          <t>138.71</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>+2.74</t>
+          <t>-0.02</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>+2.01%</t>
+          <t>-0.02%</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>7%</t>
         </is>
       </c>
     </row>
@@ -495,17 +510,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>137.58</t>
+          <t>137.65</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>+2.51</t>
+          <t>+0.07</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+1.86%</t>
+          <t>+0.05%</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>7%</t>
         </is>
       </c>
     </row>
@@ -517,17 +537,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>127.96</t>
+          <t>126.45</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>+2.00</t>
+          <t>-1.51</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+1.59%</t>
+          <t>-1.18%</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-16%</t>
         </is>
       </c>
     </row>
@@ -539,17 +564,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>315.43</t>
+          <t>316.39</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>+10.64</t>
+          <t>+0.96</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+3.49%</t>
+          <t>+0.30%</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-5%</t>
         </is>
       </c>
     </row>
@@ -561,17 +591,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>327.26</t>
+          <t>327.56</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>+7.90</t>
+          <t>+0.30</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>+2.47%</t>
+          <t>+0.09%</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-3%</t>
         </is>
       </c>
     </row>
@@ -583,17 +618,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>457.62</t>
+          <t>446.82</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>+10.74</t>
+          <t>-10.80</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>+2.40%</t>
+          <t>-2.36%</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>5%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added discord bot, django, and microsoft azure integration
</commit_message>
<xml_diff>
--- a/stockDataFile.xlsx
+++ b/stockDataFile.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -456,22 +456,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>177.70</t>
+          <t>173.80</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+0.21</t>
+          <t>+1.05</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>+0.12%</t>
+          <t>+0.61%</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-2%</t>
+          <t>-1%</t>
         </is>
       </c>
     </row>
@@ -483,22 +483,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>138.71</t>
+          <t>139.62</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-0.02</t>
+          <t>+0.68</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>-0.02%</t>
+          <t>+0.49%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>6%</t>
         </is>
       </c>
     </row>
@@ -510,22 +510,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>137.65</t>
+          <t>138.50</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>+0.07</t>
+          <t>+0.83</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+0.05%</t>
+          <t>+0.60%</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>7%</t>
+          <t>6%</t>
         </is>
       </c>
     </row>
@@ -537,22 +537,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>126.45</t>
+          <t>175.39</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-1.51</t>
+          <t>+3.43</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-1.18%</t>
+          <t>+1.99%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-16%</t>
+          <t>-5%</t>
         </is>
       </c>
     </row>
@@ -564,17 +564,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>316.39</t>
+          <t>483.59</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>+0.96</t>
+          <t>-22.36</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+0.30%</t>
+          <t>-4.42%</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -591,22 +591,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>327.56</t>
+          <t>415.28</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>+0.30</t>
+          <t>+10.76</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>+0.09%</t>
+          <t>+2.66%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-3%</t>
+          <t>-2%</t>
         </is>
       </c>
     </row>
@@ -618,22 +618,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>446.82</t>
+          <t>919.13</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-10.80</t>
+          <t>+61.39</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-2.36%</t>
+          <t>+7.16%</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>8%</t>
         </is>
       </c>
     </row>

</xml_diff>